<commit_message>
alteração de diretorio do arquivo excel
</commit_message>
<xml_diff>
--- a/Version 1-AmbienteDeTeste/ExcelTestSSO.xlsx
+++ b/Version 1-AmbienteDeTeste/ExcelTestSSO.xlsx
@@ -371,7 +371,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,16 +620,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88C4F8A-EE52-4C73-95BB-463EC08B7471}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7a4cb89e-0dcd-4fac-972d-6428dc4a4f83"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1403520b-a90b-4c50-b36b-07d0abd0460b"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7a4cb89e-0dcd-4fac-972d-6428dc4a4f83"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1403520b-a90b-4c50-b36b-07d0abd0460b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>